<commit_message>
committing updated activity report and topics.txt
</commit_message>
<xml_diff>
--- a/CDSIWAR_LMC.xlsx
+++ b/CDSIWAR_LMC.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="119">
   <si>
     <t>Week</t>
   </si>
@@ -393,6 +393,18 @@
   </si>
   <si>
     <t>D365 Development Training - Reports (Activities)</t>
+  </si>
+  <si>
+    <t>D365 Development Training - Reports (Continuation w/ Activities)</t>
+  </si>
+  <si>
+    <t>D365 Development Training - Security Basics, Data Entities</t>
+  </si>
+  <si>
+    <t>D365 Development Training - Reports (Finalization w/Activities)</t>
+  </si>
+  <si>
+    <t>D365 Development Training - Security Basics, Data Entities (Continuation w/Activities)</t>
   </si>
 </sst>
 </file>
@@ -920,7 +932,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -996,9 +1008,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2368,7 +2377,7 @@
       <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2600,7 +2609,7 @@
       <c r="J9" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="K9" s="47"/>
+      <c r="K9" s="46"/>
     </row>
     <row r="10" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
@@ -2673,7 +2682,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="32" t="str">
-        <f t="shared" ref="B12:B14" si="0">TEXT(D12,"ddd")</f>
+        <f t="shared" ref="B12" si="0">TEXT(D12,"ddd")</f>
         <v>Thu</v>
       </c>
       <c r="C12" s="12" t="s">
@@ -2902,137 +2911,213 @@
     </row>
     <row r="19" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="32">
-        <f>WEEKNUM(D19,2)</f>
-        <v>1</v>
-      </c>
-      <c r="B19" s="32" t="str">
-        <f>TEXT(D19,"ddd")</f>
-        <v>Sat</v>
-      </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
+        <v>2</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="30">
+        <v>44818</v>
+      </c>
+      <c r="E19" s="23">
+        <v>0.37638888888888888</v>
+      </c>
+      <c r="F19" s="23">
+        <v>0.5</v>
+      </c>
       <c r="G19" s="14" t="str">
         <f>TEXT((DetailsTable[[#This Row],[Time out]]-DetailsTable[[#This Row],[Time in]]),"h:mm")</f>
-        <v>0:00</v>
-      </c>
-      <c r="H19" s="17"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="15"/>
+        <v>2:58</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="20" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="13">
-        <f t="shared" ref="A20:A51" si="1">WEEKNUM(D20,2)</f>
-        <v>1</v>
-      </c>
-      <c r="B20" s="13" t="str">
-        <f t="shared" ref="B20:B51" si="2">TEXT(D20,"ddd")</f>
-        <v>Sat</v>
-      </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
+        <v>2</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="30">
+        <v>44818</v>
+      </c>
+      <c r="E20" s="34">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F20" s="34">
+        <v>0.75138888888888899</v>
+      </c>
       <c r="G20" s="14" t="str">
         <f>TEXT((DetailsTable[[#This Row],[Time out]]-DetailsTable[[#This Row],[Time in]]),"h:mm")</f>
-        <v>0:00</v>
-      </c>
-      <c r="H20" s="17"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="15"/>
+        <v>5:02</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="21" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B21" s="13" t="str">
-        <f t="shared" si="2"/>
-        <v>Sat</v>
-      </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
+        <f t="shared" ref="B20:B51" si="1">TEXT(D21,"ddd")</f>
+        <v>Thu</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="30">
+        <v>44819</v>
+      </c>
+      <c r="E21" s="23">
+        <v>0.37638888888888888</v>
+      </c>
+      <c r="F21" s="23">
+        <v>0.5</v>
+      </c>
       <c r="G21" s="14" t="str">
         <f>TEXT((DetailsTable[[#This Row],[Time out]]-DetailsTable[[#This Row],[Time in]]),"h:mm")</f>
-        <v>0:00</v>
-      </c>
-      <c r="H21" s="17"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="15"/>
+        <v>2:58</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="22" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="13">
+        <v>2</v>
+      </c>
+      <c r="B22" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B22" s="13" t="str">
-        <f t="shared" si="2"/>
-        <v>Sat</v>
-      </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
+        <v>Thu</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="30">
+        <v>44819</v>
+      </c>
+      <c r="E22" s="34">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F22" s="34">
+        <v>0.75138888888888899</v>
+      </c>
       <c r="G22" s="14" t="str">
         <f>TEXT((DetailsTable[[#This Row],[Time out]]-DetailsTable[[#This Row],[Time in]]),"h:mm")</f>
-        <v>0:00</v>
-      </c>
-      <c r="H22" s="17"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="15"/>
+        <v>5:02</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="23" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="13">
+        <v>2</v>
+      </c>
+      <c r="B23" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B23" s="13" t="str">
-        <f t="shared" si="2"/>
-        <v>Sat</v>
-      </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
+        <v>Fri</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="30">
+        <v>44820</v>
+      </c>
+      <c r="E23" s="34">
+        <v>0.3756944444444445</v>
+      </c>
+      <c r="F23" s="34">
+        <v>0.50624999999999998</v>
+      </c>
       <c r="G23" s="14" t="str">
         <f>TEXT((DetailsTable[[#This Row],[Time out]]-DetailsTable[[#This Row],[Time in]]),"h:mm")</f>
-        <v>0:00</v>
-      </c>
-      <c r="H23" s="17"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="41"/>
+        <v>3:08</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="24" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="13">
+        <v>2</v>
+      </c>
+      <c r="B24" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B24" s="13" t="str">
-        <f t="shared" si="2"/>
-        <v>Sat</v>
-      </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
+        <v>Fri</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="30">
+        <v>44820</v>
+      </c>
+      <c r="E24" s="34">
+        <v>0.55347222222222225</v>
+      </c>
+      <c r="F24" s="34">
+        <v>0.75694444444444453</v>
+      </c>
       <c r="G24" s="14" t="str">
         <f>TEXT((DetailsTable[[#This Row],[Time out]]-DetailsTable[[#This Row],[Time in]]),"h:mm")</f>
-        <v>0:00</v>
-      </c>
-      <c r="H24" s="17"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="15"/>
+        <v>4:53</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J24" s="15" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="25" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="13">
+        <f t="shared" ref="A20:A51" si="2">WEEKNUM(D25,2)</f>
+        <v>1</v>
+      </c>
+      <c r="B25" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B25" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C25" s="12"/>
@@ -3046,18 +3131,18 @@
       <c r="H25" s="17"/>
       <c r="I25" s="12"/>
       <c r="J25" s="15"/>
-      <c r="K25" s="46">
+      <c r="K25" s="45">
         <f>SUM(G4:G19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B26" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B26" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C26" s="12"/>
@@ -3074,11 +3159,11 @@
     </row>
     <row r="27" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B27" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B27" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C27" s="12"/>
@@ -3095,11 +3180,11 @@
     </row>
     <row r="28" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B28" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B28" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C28" s="12"/>
@@ -3116,11 +3201,11 @@
     </row>
     <row r="29" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B29" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B29" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C29" s="12"/>
@@ -3137,11 +3222,11 @@
     </row>
     <row r="30" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B30" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B30" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C30" s="12"/>
@@ -3158,11 +3243,11 @@
     </row>
     <row r="31" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B31" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B31" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C31" s="12"/>
@@ -3179,11 +3264,11 @@
     </row>
     <row r="32" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B32" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B32" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C32" s="12"/>
@@ -3200,11 +3285,11 @@
     </row>
     <row r="33" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B33" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B33" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C33" s="12"/>
@@ -3221,32 +3306,32 @@
     </row>
     <row r="34" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B34" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B34" s="13" t="str">
-        <f t="shared" si="2"/>
-        <v>Sat</v>
-      </c>
-      <c r="C34" s="43"/>
+        <v>Sat</v>
+      </c>
+      <c r="C34" s="42"/>
       <c r="D34" s="28"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="44"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
       <c r="G34" s="14" t="str">
         <f>TEXT((DetailsTable[[#This Row],[Time out]]-DetailsTable[[#This Row],[Time in]]),"h:mm")</f>
         <v>0:00</v>
       </c>
-      <c r="H34" s="45"/>
-      <c r="I34" s="43"/>
-      <c r="J34" s="42"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="42"/>
+      <c r="J34" s="41"/>
     </row>
     <row r="35" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B35" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B35" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C35" s="12"/>
@@ -3263,11 +3348,11 @@
     </row>
     <row r="36" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B36" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B36" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C36" s="12"/>
@@ -3281,7 +3366,7 @@
       <c r="H36" s="17"/>
       <c r="I36" s="12"/>
       <c r="J36" s="21"/>
-      <c r="L36" s="46">
+      <c r="L36" s="45">
         <f>SUM(G4:G29)</f>
         <v>0</v>
       </c>
@@ -3306,18 +3391,18 @@
       <c r="H37" s="17"/>
       <c r="I37" s="12"/>
       <c r="J37" s="39"/>
-      <c r="L37" s="46">
+      <c r="L37" s="45">
         <f>SUM(G4:G29)</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B38" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B38" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C38" s="12"/>
@@ -3334,11 +3419,11 @@
     </row>
     <row r="39" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B39" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B39" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C39" s="12"/>
@@ -3355,11 +3440,11 @@
     </row>
     <row r="40" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B40" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B40" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C40" s="12"/>
@@ -3376,11 +3461,11 @@
     </row>
     <row r="41" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B41" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B41" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C41" s="12"/>
@@ -3397,11 +3482,11 @@
     </row>
     <row r="42" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B42" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B42" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C42" s="12"/>
@@ -3418,11 +3503,11 @@
     </row>
     <row r="43" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B43" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B43" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C43" s="12"/>
@@ -3439,11 +3524,11 @@
     </row>
     <row r="44" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B44" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B44" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C44" s="12"/>
@@ -3460,11 +3545,11 @@
     </row>
     <row r="45" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B45" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B45" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C45" s="12"/>
@@ -3481,11 +3566,11 @@
     </row>
     <row r="46" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B46" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B46" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C46" s="12"/>
@@ -3502,11 +3587,11 @@
     </row>
     <row r="47" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B47" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B47" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C47" s="12"/>
@@ -3523,11 +3608,11 @@
     </row>
     <row r="48" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B48" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B48" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C48" s="12"/>
@@ -3544,11 +3629,11 @@
     </row>
     <row r="49" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B49" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B49" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C49" s="12"/>
@@ -3565,11 +3650,11 @@
     </row>
     <row r="50" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B50" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B50" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C50" s="12"/>
@@ -3586,11 +3671,11 @@
     </row>
     <row r="51" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B51" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B51" s="13" t="str">
-        <f t="shared" si="2"/>
         <v>Sat</v>
       </c>
       <c r="C51" s="12"/>
@@ -15137,6 +15222,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F617D5D6C2326244B945A153B2699D83" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="729ff3d1dfa1b0e3159d7adc89176057">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cfde720a-0586-4dda-8f1e-44106db839b2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="75fdde4a3c23aebaadb6d43fc9a28e41" ns2:_="">
     <xsd:import namespace="cfde720a-0586-4dda-8f1e-44106db839b2"/>
@@ -15280,22 +15380,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74F0C21E-798F-42EB-93E2-07F38EACDD56}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cfde720a-0586-4dda-8f1e-44106db839b2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B01623-99F0-4F5F-87D1-E6F1F0AA2529}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A937C81F-37D0-49D9-BB44-3922ADAA15B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15311,28 +15420,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B01623-99F0-4F5F-87D1-E6F1F0AA2529}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74F0C21E-798F-42EB-93E2-07F38EACDD56}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cfde720a-0586-4dda-8f1e-44106db839b2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
committing updated WAR, topics, images, and development training ntoes
</commit_message>
<xml_diff>
--- a/CDSIWAR_LMC.xlsx
+++ b/CDSIWAR_LMC.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="129">
   <si>
     <t>Week</t>
   </si>
@@ -420,6 +420,21 @@
   </si>
   <si>
     <t>D365 Development Training - Data Entities (Finalization w/Activities)</t>
+  </si>
+  <si>
+    <t>D365 Development Training - Power BI (Finalization w/Activities)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D365 Development Training - Exporting Projects </t>
+  </si>
+  <si>
+    <t>D365 Development Training - Exporting Projects (Continuation)</t>
+  </si>
+  <si>
+    <t>RLC - Customer Aging Report - Commercial Setup</t>
+  </si>
+  <si>
+    <t>RLC - Customer Aging Report - Commercial Setup (Continuation)</t>
   </si>
 </sst>
 </file>
@@ -947,7 +962,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1031,9 +1046,6 @@
     </xf>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -2389,10 +2401,10 @@
   <dimension ref="A3:T391"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="F13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomRight" activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2624,7 +2636,7 @@
       <c r="J9" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="K9" s="46"/>
+      <c r="K9" s="45"/>
     </row>
     <row r="10" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
@@ -3158,7 +3170,7 @@
       <c r="J25" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="K25" s="45">
+      <c r="K25" s="44">
         <f>SUM(G4:G19)</f>
         <v>0</v>
       </c>
@@ -3279,11 +3291,11 @@
         <v>0.3756944444444445</v>
       </c>
       <c r="F29" s="34">
-        <v>0.54166666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="G29" s="14" t="str">
         <f>TEXT((DetailsTable[[#This Row],[Time out]]-DetailsTable[[#This Row],[Time in]]),"h:mm")</f>
-        <v>3:59</v>
+        <v>2:59</v>
       </c>
       <c r="H29" s="17" t="s">
         <v>15</v>
@@ -3308,142 +3320,224 @@
       <c r="D30" s="28">
         <v>44825</v>
       </c>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
+      <c r="E30" s="34">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F30" s="34">
+        <v>0.76458333333333339</v>
+      </c>
       <c r="G30" s="14" t="str">
         <f>TEXT((DetailsTable[[#This Row],[Time out]]-DetailsTable[[#This Row],[Time in]]),"h:mm")</f>
-        <v>0:00</v>
-      </c>
-      <c r="H30" s="17"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="21"/>
+        <v>5:21</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J30" s="21" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="31" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="13">
-        <f t="shared" ref="A28:A51" si="2">WEEKNUM(D31,2)</f>
-        <v>1</v>
-      </c>
-      <c r="B31" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>Sat</v>
-      </c>
-      <c r="C31" s="12"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
+        <v>3</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="28">
+        <v>44826</v>
+      </c>
+      <c r="E31" s="34">
+        <v>0.375</v>
+      </c>
+      <c r="F31" s="34">
+        <v>0.5</v>
+      </c>
       <c r="G31" s="14" t="str">
         <f>TEXT((DetailsTable[[#This Row],[Time out]]-DetailsTable[[#This Row],[Time in]]),"h:mm")</f>
-        <v>0:00</v>
-      </c>
-      <c r="H31" s="17"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="21"/>
+        <v>3:00</v>
+      </c>
+      <c r="H31" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J31" s="21" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="32" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="13">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="B32" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>Sat</v>
-      </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
+        <v>3</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="28">
+        <v>44826</v>
+      </c>
+      <c r="E32" s="34">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F32" s="34">
+        <v>0.75</v>
+      </c>
       <c r="G32" s="14" t="str">
         <f>TEXT((DetailsTable[[#This Row],[Time out]]-DetailsTable[[#This Row],[Time in]]),"h:mm")</f>
-        <v>0:00</v>
-      </c>
-      <c r="H32" s="17"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="21"/>
+        <v>5:00</v>
+      </c>
+      <c r="H32" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J32" s="21" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="33" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="13">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="B33" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>Sat</v>
-      </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
+        <v>3</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" s="28">
+        <v>44827</v>
+      </c>
+      <c r="E33" s="34">
+        <v>0.375</v>
+      </c>
+      <c r="F33" s="34">
+        <v>0.5</v>
+      </c>
       <c r="G33" s="14" t="str">
         <f>TEXT((DetailsTable[[#This Row],[Time out]]-DetailsTable[[#This Row],[Time in]]),"h:mm")</f>
-        <v>0:00</v>
-      </c>
-      <c r="H33" s="17"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="21"/>
+        <v>3:00</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J33" s="21" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="34" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="13">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="B34" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>Sat</v>
-      </c>
-      <c r="C34" s="42"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
+        <v>3</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" s="28">
+        <v>44827</v>
+      </c>
+      <c r="E34" s="43">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F34" s="43">
+        <v>0.76388888888888884</v>
+      </c>
       <c r="G34" s="14" t="str">
         <f>TEXT((DetailsTable[[#This Row],[Time out]]-DetailsTable[[#This Row],[Time in]]),"h:mm")</f>
-        <v>0:00</v>
-      </c>
-      <c r="H34" s="44"/>
-      <c r="I34" s="42"/>
-      <c r="J34" s="41"/>
+        <v>5:20</v>
+      </c>
+      <c r="H34" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J34" s="41" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="35" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="13">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="B35" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>Sat</v>
-      </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
+        <v>4</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" s="28">
+        <v>44830</v>
+      </c>
+      <c r="E35" s="34">
+        <v>0.375</v>
+      </c>
+      <c r="F35" s="34">
+        <v>0.5</v>
+      </c>
       <c r="G35" s="14" t="str">
         <f>TEXT((DetailsTable[[#This Row],[Time out]]-DetailsTable[[#This Row],[Time in]]),"h:mm")</f>
-        <v>0:00</v>
-      </c>
-      <c r="H35" s="17"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="21"/>
+        <v>3:00</v>
+      </c>
+      <c r="H35" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J35" s="41" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="36" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="13">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="B36" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v>Sat</v>
-      </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+        <v>4</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" s="28">
+        <v>44830</v>
+      </c>
+      <c r="E36" s="34">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F36" s="34">
+        <v>0.75416666666666676</v>
+      </c>
       <c r="G36" s="14" t="str">
         <f>TEXT((DetailsTable[[#This Row],[Time out]]-DetailsTable[[#This Row],[Time in]]),"h:mm")</f>
-        <v>0:00</v>
-      </c>
-      <c r="H36" s="17"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="21"/>
-      <c r="L36" s="45">
+        <v>5:06</v>
+      </c>
+      <c r="H36" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J36" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="L36" s="44">
         <f>SUM(G4:G29)</f>
         <v>0</v>
       </c>
@@ -3468,14 +3562,14 @@
       <c r="H37" s="17"/>
       <c r="I37" s="12"/>
       <c r="J37" s="39"/>
-      <c r="L37" s="45">
+      <c r="L37" s="44">
         <f>SUM(G4:G29)</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="A31:A51" si="2">WEEKNUM(D38,2)</f>
         <v>1</v>
       </c>
       <c r="B38" s="13" t="str">
@@ -15299,6 +15393,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F617D5D6C2326244B945A153B2699D83" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="729ff3d1dfa1b0e3159d7adc89176057">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cfde720a-0586-4dda-8f1e-44106db839b2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="75fdde4a3c23aebaadb6d43fc9a28e41" ns2:_="">
     <xsd:import namespace="cfde720a-0586-4dda-8f1e-44106db839b2"/>
@@ -15442,22 +15551,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74F0C21E-798F-42EB-93E2-07F38EACDD56}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cfde720a-0586-4dda-8f1e-44106db839b2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B01623-99F0-4F5F-87D1-E6F1F0AA2529}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A937C81F-37D0-49D9-BB44-3922ADAA15B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15473,28 +15591,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B01623-99F0-4F5F-87D1-E6F1F0AA2529}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74F0C21E-798F-42EB-93E2-07F38EACDD56}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cfde720a-0586-4dda-8f1e-44106db839b2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
final commit after finishing internship
</commit_message>
<xml_diff>
--- a/CDSIWAR_LMC.xlsx
+++ b/CDSIWAR_LMC.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="157">
   <si>
     <t>Week</t>
   </si>
@@ -513,6 +513,12 @@
   </si>
   <si>
     <t>RLC - Customer Aging Report - Updated report temporary table for report layout</t>
+  </si>
+  <si>
+    <t>RLC - Customer Aging Report - Placed conditions for transactions to which aging bucket it will fall under</t>
+  </si>
+  <si>
+    <t>RLC - Customer Aging Report - Placed conditions for transactions to which aging bucket it will fall under (Continuation)</t>
   </si>
 </sst>
 </file>
@@ -2445,10 +2451,10 @@
   <dimension ref="A3:T391"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="F18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J62" sqref="J62"/>
+      <selection pane="bottomRight" activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4446,51 +4452,74 @@
         <v>154</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A63" s="13">
-        <f t="shared" ref="A61:A83" si="3">WEEKNUM(D63,2)</f>
-        <v>1</v>
-      </c>
-      <c r="B63" s="13" t="str">
-        <f t="shared" si="2"/>
-        <v>Sat</v>
-      </c>
-      <c r="C63" s="12"/>
-      <c r="D63" s="28"/>
-      <c r="E63" s="34"/>
-      <c r="F63" s="34"/>
+        <v>6</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D63" s="28">
+        <v>44848</v>
+      </c>
+      <c r="E63" s="34">
+        <v>0.375</v>
+      </c>
+      <c r="F63" s="34">
+        <v>0.54861111111111105</v>
+      </c>
       <c r="G63" s="14" t="str">
         <f>TEXT((DetailsTable[[#This Row],[Time out]]-DetailsTable[[#This Row],[Time in]]),"h:mm")</f>
-        <v>0:00</v>
-      </c>
-      <c r="H63" s="17"/>
-      <c r="I63" s="12"/>
-      <c r="J63" s="21"/>
-    </row>
-    <row r="64" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+        <v>4:10</v>
+      </c>
+      <c r="H63" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I63" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J63" s="21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A64" s="13">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="B64" s="13" t="str">
-        <f t="shared" si="2"/>
-        <v>Sat</v>
-      </c>
-      <c r="C64" s="12"/>
-      <c r="D64" s="28"/>
-      <c r="E64" s="34"/>
-      <c r="F64" s="34"/>
+        <v>6</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D64" s="28">
+        <v>44848</v>
+      </c>
+      <c r="E64" s="34">
+        <v>0.59375</v>
+      </c>
+      <c r="F64" s="34">
+        <v>0.75208333333333333</v>
+      </c>
       <c r="G64" s="14" t="str">
         <f>TEXT((DetailsTable[[#This Row],[Time out]]-DetailsTable[[#This Row],[Time in]]),"h:mm")</f>
-        <v>0:00</v>
-      </c>
-      <c r="H64" s="17"/>
-      <c r="I64" s="12"/>
-      <c r="J64" s="21"/>
+        <v>3:48</v>
+      </c>
+      <c r="H64" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I64" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J64" s="21" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="65" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="13">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="B65" s="13" t="str">
@@ -4511,7 +4540,7 @@
     </row>
     <row r="66" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="A63:A83" si="3">WEEKNUM(D66,2)</f>
         <v>1</v>
       </c>
       <c r="B66" s="13" t="str">
@@ -15747,6 +15776,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F617D5D6C2326244B945A153B2699D83" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="729ff3d1dfa1b0e3159d7adc89176057">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cfde720a-0586-4dda-8f1e-44106db839b2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="75fdde4a3c23aebaadb6d43fc9a28e41" ns2:_="">
     <xsd:import namespace="cfde720a-0586-4dda-8f1e-44106db839b2"/>
@@ -15890,12 +15925,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -15906,6 +15935,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74F0C21E-798F-42EB-93E2-07F38EACDD56}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cfde720a-0586-4dda-8f1e-44106db839b2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A937C81F-37D0-49D9-BB44-3922ADAA15B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15923,22 +15968,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74F0C21E-798F-42EB-93E2-07F38EACDD56}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cfde720a-0586-4dda-8f1e-44106db839b2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B01623-99F0-4F5F-87D1-E6F1F0AA2529}">
   <ds:schemaRefs>

</xml_diff>